<commit_message>
Mettre à jour scrum #1
</commit_message>
<xml_diff>
--- a/scrum/sprint_1.xlsx
+++ b/scrum/sprint_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Documents/L2/013/ForestWorld/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Documents/L2/013/ForestWorld/scrum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B292DA43-E2DF-B146-B29C-E513ACE8E0CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7180161-8536-B545-AA3C-36AD058EB69F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-500" yWindow="500" windowWidth="27640" windowHeight="16440" xr2:uid="{73087F09-11BA-DA46-A1D1-CF04ABE318B5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27640" windowHeight="16440" xr2:uid="{73087F09-11BA-DA46-A1D1-CF04ABE318B5}"/>
   </bookViews>
   <sheets>
     <sheet name="semaine_1" sheetId="1" r:id="rId1"/>
@@ -1344,8 +1344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BC1C68-DB6D-104B-A89E-FD56C0ED0445}">
   <dimension ref="A1:AD230"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1624,10 +1624,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="67"/>
-      <c r="F8" s="67" t="s">
+      <c r="F8" s="67"/>
+      <c r="G8" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="68"/>
       <c r="H8" s="69"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>

</xml_diff>

<commit_message>
mise à jour de sprint 1
Signed-off-by: Tristan Charpentier <tristan_charpentier@hotmail.com>
</commit_message>
<xml_diff>
--- a/scrum/sprint_1.xlsx
+++ b/scrum/sprint_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Documents/L2/013/ForestWorld/scrum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7180161-8536-B545-AA3C-36AD058EB69F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E27967-9E36-494E-99B3-9DE80EC7A5CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27640" windowHeight="16440" xr2:uid="{73087F09-11BA-DA46-A1D1-CF04ABE318B5}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>En attente</t>
   </si>
@@ -1344,8 +1344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BC1C68-DB6D-104B-A89E-FD56C0ED0445}">
   <dimension ref="A1:AD230"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:G22"/>
+    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="156" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1474,7 +1474,9 @@
       <c r="E4" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="59"/>
+      <c r="F4" s="59" t="s">
+        <v>3</v>
+      </c>
       <c r="G4" s="60"/>
       <c r="H4" s="61"/>
       <c r="I4" s="3"/>

</xml_diff>

<commit_message>
mise à jour de scrum
Signed-off-by: Tristan Charpentier <tristan_charpentier@hotmail.com>
</commit_message>
<xml_diff>
--- a/scrum/sprint_1.xlsx
+++ b/scrum/sprint_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Documents/L2/013/ForestWorld/scrum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E27967-9E36-494E-99B3-9DE80EC7A5CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B27479-9BC7-D849-9541-09B43E722AA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27640" windowHeight="16440" xr2:uid="{73087F09-11BA-DA46-A1D1-CF04ABE318B5}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
   <si>
     <t>En attente</t>
   </si>
@@ -1344,8 +1344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BC1C68-DB6D-104B-A89E-FD56C0ED0445}">
   <dimension ref="A1:AD230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="156" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="113" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1471,9 +1471,7 @@
       <c r="D4" s="58">
         <v>2</v>
       </c>
-      <c r="E4" s="59" t="s">
-        <v>3</v>
-      </c>
+      <c r="E4" s="59"/>
       <c r="F4" s="59" t="s">
         <v>3</v>
       </c>
@@ -1549,10 +1547,10 @@
       <c r="D6" s="58">
         <v>2</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="59"/>
+      <c r="F6" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="59"/>
       <c r="G6" s="60"/>
       <c r="H6" s="61"/>
       <c r="I6" s="3"/>
@@ -1937,10 +1935,10 @@
       <c r="D16" s="58">
         <v>2</v>
       </c>
-      <c r="E16" s="59" t="s">
+      <c r="E16" s="59"/>
+      <c r="F16" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="59"/>
       <c r="G16" s="60"/>
       <c r="H16" s="61"/>
       <c r="I16" s="3"/>

</xml_diff>

<commit_message>
amélioration de la fonction de rendu (4x plus performant)
Signed-off-by: Tristan Charpentier <tristan_charpentier@hotmail.com>
</commit_message>
<xml_diff>
--- a/scrum/sprint_1.xlsx
+++ b/scrum/sprint_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Documents/L2/013/ForestWorld/scrum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B27479-9BC7-D849-9541-09B43E722AA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93A5915-528D-CA42-9832-10D4CB226E60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27640" windowHeight="16440" xr2:uid="{73087F09-11BA-DA46-A1D1-CF04ABE318B5}"/>
   </bookViews>
@@ -1344,7 +1344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BC1C68-DB6D-104B-A89E-FD56C0ED0445}">
   <dimension ref="A1:AD230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="113" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -1779,11 +1779,11 @@
       <c r="D12" s="74">
         <v>1</v>
       </c>
-      <c r="E12" s="75" t="s">
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="75"/>
-      <c r="G12" s="76"/>
       <c r="H12" s="77"/>
       <c r="I12" s="25"/>
       <c r="J12" s="25"/>

</xml_diff>

<commit_message>
impl de la caméra
Signed-off-by: Tristan Charpentier <tristan_charpentier@hotmail.com>
</commit_message>
<xml_diff>
--- a/scrum/sprint_1.xlsx
+++ b/scrum/sprint_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Documents/L2/013/ForestWorld/scrum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93A5915-528D-CA42-9832-10D4CB226E60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B682ED01-04EB-6345-BA2A-77E96D873EB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27640" windowHeight="16440" xr2:uid="{73087F09-11BA-DA46-A1D1-CF04ABE318B5}"/>
   </bookViews>
@@ -1344,8 +1344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BC1C68-DB6D-104B-A89E-FD56C0ED0445}">
   <dimension ref="A1:AD230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1510,10 +1510,10 @@
         <v>1</v>
       </c>
       <c r="E5" s="59"/>
-      <c r="F5" s="59" t="s">
+      <c r="F5" s="59"/>
+      <c r="G5" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="60"/>
       <c r="H5" s="61"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -1936,10 +1936,10 @@
         <v>2</v>
       </c>
       <c r="E16" s="59"/>
-      <c r="F16" s="59" t="s">
+      <c r="F16" s="59"/>
+      <c r="G16" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="60"/>
       <c r="H16" s="61"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
@@ -1973,11 +1973,11 @@
       <c r="D17" s="66">
         <v>3</v>
       </c>
-      <c r="E17" s="67" t="s">
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="67"/>
-      <c r="G17" s="68"/>
       <c r="H17" s="69"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>

</xml_diff>